<commit_message>
finalized project included final report
</commit_message>
<xml_diff>
--- a/Report/report table.xlsx
+++ b/Report/report table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AJ-CPU\Documents\GitHub\pollinator-strip-runoff\Report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5840720E-B93D-4C27-B9DA-9FF2606058CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F11491AC-B157-4E41-8BF1-30A47BE21E5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="5280" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$50:$F$59</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$I$28:$M$37</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="47">
   <si>
     <t>Nitrogen, Nitrate (As N)</t>
   </si>
@@ -186,8 +186,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0.0E+00"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="0.0E+00"/>
+    <numFmt numFmtId="166" formatCode="0.0"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -206,7 +207,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -214,15 +215,48 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -505,10 +539,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A4:K62"/>
+  <dimension ref="A4:M47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="B50" sqref="B50:F62"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="I49" sqref="I49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -516,6 +550,8 @@
     <col min="2" max="2" width="20.86328125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="37.796875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="37.796875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="1:11" x14ac:dyDescent="0.45">
@@ -955,7 +991,7 @@
         <v>84.885458999999997</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A17">
         <v>13</v>
       </c>
@@ -990,7 +1026,7 @@
         <v>-11.533396</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A18">
         <v>14</v>
       </c>
@@ -1025,7 +1061,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A19">
         <v>15</v>
       </c>
@@ -1060,7 +1096,7 @@
         <v>-83.908045999999999</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A20">
         <v>16</v>
       </c>
@@ -1095,7 +1131,7 @@
         <v>59.201473999999997</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A21">
         <v>17</v>
       </c>
@@ -1130,7 +1166,7 @@
         <v>-321.78217799999999</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A22">
         <v>18</v>
       </c>
@@ -1165,7 +1201,7 @@
         <v>-47.813555999999998</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A23">
         <v>19</v>
       </c>
@@ -1200,7 +1236,7 @@
         <v>67.917345999999995</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.45">
       <c r="D27" t="s">
         <v>19</v>
       </c>
@@ -1211,7 +1247,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.45">
       <c r="B28" t="s">
         <v>15</v>
       </c>
@@ -1227,8 +1263,23 @@
       <c r="F28" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="I28" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="J28" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="K28" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="L28" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="M28" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.45">
       <c r="B29">
         <v>2021</v>
       </c>
@@ -1247,8 +1298,23 @@
         <f>ROUND(K5,2)</f>
         <v>8.02</v>
       </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="I29" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="J29" s="3">
+        <v>2021</v>
+      </c>
+      <c r="K29" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="L29" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="M29" s="4">
+        <v>8.02</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.45">
       <c r="B30">
         <v>2021</v>
       </c>
@@ -1267,8 +1333,21 @@
         <f t="shared" ref="F30:F47" si="2">ROUND(K6,2)</f>
         <v>28.48</v>
       </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="I30" s="5"/>
+      <c r="J30" s="3">
+        <v>2022</v>
+      </c>
+      <c r="K30" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="L30" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="M30" s="4">
+        <v>10.93</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.45">
       <c r="B31">
         <v>2021</v>
       </c>
@@ -1287,8 +1366,21 @@
         <f t="shared" si="2"/>
         <v>-2.73</v>
       </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="I31" s="5"/>
+      <c r="J31" s="3">
+        <v>2023</v>
+      </c>
+      <c r="K31" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="L31" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="M31" s="4">
+        <v>-11.53</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.45">
       <c r="B32">
         <v>2021</v>
       </c>
@@ -1307,8 +1399,23 @@
         <f t="shared" si="2"/>
         <v>-2.79</v>
       </c>
-    </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="I32" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="J32" s="3">
+        <v>2021</v>
+      </c>
+      <c r="K32" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="L32" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="M32" s="4">
+        <v>28.48</v>
+      </c>
+    </row>
+    <row r="33" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B33">
         <v>2021</v>
       </c>
@@ -1327,8 +1434,21 @@
         <f t="shared" si="2"/>
         <v>57.67</v>
       </c>
-    </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="I33" s="5"/>
+      <c r="J33" s="3">
+        <v>2022</v>
+      </c>
+      <c r="K33" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="L33" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="M33" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="34" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B34">
         <v>2022</v>
       </c>
@@ -1347,8 +1467,21 @@
         <f t="shared" si="2"/>
         <v>10.93</v>
       </c>
-    </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="I34" s="5"/>
+      <c r="J34" s="3">
+        <v>2023</v>
+      </c>
+      <c r="K34" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="L34" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="M34" s="4">
+        <v>-83.91</v>
+      </c>
+    </row>
+    <row r="35" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B35">
         <v>2022</v>
       </c>
@@ -1367,8 +1500,23 @@
         <f t="shared" si="2"/>
         <v>-4.55</v>
       </c>
-    </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="I35" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="J35" s="3">
+        <v>2021</v>
+      </c>
+      <c r="K35" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="L35" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="M35" s="4">
+        <v>-2.73</v>
+      </c>
+    </row>
+    <row r="36" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B36">
         <v>2022</v>
       </c>
@@ -1387,8 +1535,21 @@
         <f t="shared" si="2"/>
         <v>#VALUE!</v>
       </c>
-    </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="I36" s="5"/>
+      <c r="J36" s="3">
+        <v>2022</v>
+      </c>
+      <c r="K36" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="L36" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="M36" s="4">
+        <v>13.69</v>
+      </c>
+    </row>
+    <row r="37" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B37">
         <v>2022</v>
       </c>
@@ -1407,8 +1568,21 @@
         <f t="shared" si="2"/>
         <v>13.69</v>
       </c>
-    </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="I37" s="5"/>
+      <c r="J37" s="3">
+        <v>2023</v>
+      </c>
+      <c r="K37" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="L37" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="M37" s="4">
+        <v>59.2</v>
+      </c>
+    </row>
+    <row r="38" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B38">
         <v>2022</v>
       </c>
@@ -1427,8 +1601,23 @@
         <f t="shared" si="2"/>
         <v>-60.32</v>
       </c>
-    </row>
-    <row r="39" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="I38" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="J38" s="8">
+        <v>2021</v>
+      </c>
+      <c r="K38" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="L38" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="M38" s="9">
+        <v>57.67</v>
+      </c>
+    </row>
+    <row r="39" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B39">
         <v>2022</v>
       </c>
@@ -1447,8 +1636,21 @@
         <f t="shared" si="2"/>
         <v>7.67</v>
       </c>
-    </row>
-    <row r="40" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="I39" s="7"/>
+      <c r="J39" s="8">
+        <v>2022</v>
+      </c>
+      <c r="K39" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="L39" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="M39" s="9">
+        <v>84.89</v>
+      </c>
+    </row>
+    <row r="40" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B40">
         <v>2022</v>
       </c>
@@ -1467,8 +1669,21 @@
         <f t="shared" si="2"/>
         <v>84.89</v>
       </c>
-    </row>
-    <row r="41" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="I40" s="10"/>
+      <c r="J40" s="6">
+        <v>2023</v>
+      </c>
+      <c r="K40" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="L40" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="M40" s="11">
+        <v>67.92</v>
+      </c>
+    </row>
+    <row r="41" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B41">
         <v>2023</v>
       </c>
@@ -1488,7 +1703,7 @@
         <v>-11.53</v>
       </c>
     </row>
-    <row r="42" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="42" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B42">
         <v>2023</v>
       </c>
@@ -1508,7 +1723,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="43" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="43" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B43">
         <v>2023</v>
       </c>
@@ -1528,7 +1743,7 @@
         <v>-83.91</v>
       </c>
     </row>
-    <row r="44" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="44" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B44">
         <v>2023</v>
       </c>
@@ -1548,7 +1763,7 @@
         <v>59.2</v>
       </c>
     </row>
-    <row r="45" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="45" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B45">
         <v>2023</v>
       </c>
@@ -1568,7 +1783,7 @@
         <v>-321.77999999999997</v>
       </c>
     </row>
-    <row r="46" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="46" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B46">
         <v>2023</v>
       </c>
@@ -1588,7 +1803,7 @@
         <v>-47.81</v>
       </c>
     </row>
-    <row r="47" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="47" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B47">
         <v>2023</v>
       </c>
@@ -1608,233 +1823,13 @@
         <v>67.92</v>
       </c>
     </row>
-    <row r="50" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="B50" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C50" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D50" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E50" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F50" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="51" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="B51" s="3">
-        <v>2021</v>
-      </c>
-      <c r="C51" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D51" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E51" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="F51" s="3">
-        <v>8.02</v>
-      </c>
-    </row>
-    <row r="52" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="B52" s="3">
-        <v>2022</v>
-      </c>
-      <c r="C52" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D52" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E52" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="F52" s="3">
-        <v>10.93</v>
-      </c>
-    </row>
-    <row r="53" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="B53" s="3">
-        <v>2023</v>
-      </c>
-      <c r="C53" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D53" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="E53" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="F53" s="3">
-        <v>-11.53</v>
-      </c>
-    </row>
-    <row r="54" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="B54" s="3">
-        <v>2021</v>
-      </c>
-      <c r="C54" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D54" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E54" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="F54" s="3">
-        <v>28.48</v>
-      </c>
-    </row>
-    <row r="55" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="B55" s="3">
-        <v>2022</v>
-      </c>
-      <c r="C55" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D55" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E55" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="F55" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="56" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="B56" s="3">
-        <v>2023</v>
-      </c>
-      <c r="C56" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D56" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E56" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="F56" s="3">
-        <v>-83.91</v>
-      </c>
-    </row>
-    <row r="57" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="B57" s="3">
-        <v>2021</v>
-      </c>
-      <c r="C57" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D57" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E57" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F57" s="3">
-        <v>-2.73</v>
-      </c>
-    </row>
-    <row r="58" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="B58" s="3">
-        <v>2022</v>
-      </c>
-      <c r="C58" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D58" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="E58" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="F58" s="3">
-        <v>13.69</v>
-      </c>
-    </row>
-    <row r="59" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="B59" s="3">
-        <v>2023</v>
-      </c>
-      <c r="C59" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D59" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="E59" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="F59" s="3">
-        <v>59.2</v>
-      </c>
-    </row>
-    <row r="60" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="B60" s="3">
-        <v>2021</v>
-      </c>
-      <c r="C60" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D60" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E60" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="F60" s="3">
-        <v>57.67</v>
-      </c>
-    </row>
-    <row r="61" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="B61" s="3">
-        <v>2022</v>
-      </c>
-      <c r="C61" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D61" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="E61" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="F61" s="3">
-        <v>84.89</v>
-      </c>
-    </row>
-    <row r="62" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="B62" s="3">
-        <v>2023</v>
-      </c>
-      <c r="C62" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D62" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="E62" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="F62" s="3">
-        <v>67.92</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="B50:F59" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B51:F62">
-      <sortCondition ref="C50:C59"/>
-    </sortState>
-  </autoFilter>
+  <mergeCells count="4">
+    <mergeCell ref="I29:I31"/>
+    <mergeCell ref="I32:I34"/>
+    <mergeCell ref="I35:I37"/>
+    <mergeCell ref="I38:I40"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>